<commit_message>
bergo update: git seemed to be stuck on a previous commit which held >100MB files, I resetted just before that.now I add my files and I attempt to push
</commit_message>
<xml_diff>
--- a/docs/docs_I_made/ebordron_review_packages_R__02_03_2022.xlsx
+++ b/docs/docs_I_made/ebordron_review_packages_R__02_03_2022.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14385" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14385"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,32 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>jc</author>
+  </authors>
+  <commentList>
+    <comment ref="F91" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">07/03: la liste des SNP probes utilisées pour calculer le GC score
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="219">
   <si>
     <t>oncoscanR</t>
   </si>
@@ -52,9 +76,6 @@
   </si>
   <si>
     <t>CEL files, only</t>
-  </si>
-  <si>
-    <t>resolution</t>
   </si>
   <si>
     <t>platform</t>
@@ -523,38 +544,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Affymetrix SNP6.0 and cytoScanHD files: 
-- probeset.txt,
-- cychp.txt
-- cnchp.txt . 
-They are exported from ChAS or Affymetrix Power Tools.
-rCGH also supports custom arrays, but we need data from a cnchp file to build it. </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CF. tableau 3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
     <t>CF. tableau 4</t>
   </si>
   <si>
@@ -738,18 +727,152 @@
     </r>
   </si>
   <si>
-    <t>objet R: cghSeg
+    <t>input de GISTIC</t>
+  </si>
+  <si>
+    <t>in cnchp files</t>
+  </si>
+  <si>
+    <t>in filename.segments.txt</t>
+  </si>
+  <si>
+    <t>( format:  CBS output)</t>
+  </si>
+  <si>
+    <t>File extension/type</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>reference-file</t>
+  </si>
+  <si>
+    <t>REF_MODEL (HDF5)</t>
+  </si>
+  <si>
+    <t>Reference data generated by apt-copynumber-onco-ref</t>
+  </si>
+  <si>
+    <t>snp-qc-snp-list</t>
+  </si>
+  <si>
+    <t>txt</t>
+  </si>
+  <si>
+    <t>SNP probes used in calculating SNP QC</t>
+  </si>
+  <si>
+    <t>annotation-file</t>
+  </si>
+  <si>
+    <t>annot.db (SQLite)</t>
+  </si>
+  <si>
+    <t>Annotation data for probes and probesets</t>
+  </si>
+  <si>
+    <t>x-probes-file</t>
+  </si>
+  <si>
+    <t>chrXprobes (text)</t>
+  </si>
+  <si>
+    <t>List of X-chromosome probes</t>
+  </si>
+  <si>
+    <t>y-probes-file</t>
+  </si>
+  <si>
+    <t>chrYprobes (text)</t>
+  </si>
+  <si>
+    <t>List of Y-chromosome probes</t>
+  </si>
+  <si>
+    <t>cel-pairs-file</t>
+  </si>
+  <si>
+    <t>tsv</t>
+  </si>
+  <si>
+    <t>Cel file pairs (AT and GC channel for each sample) for experiments</t>
+  </si>
+  <si>
+    <t>tableau 7</t>
+  </si>
+  <si>
+    <t>Actual name</t>
+  </si>
+  <si>
+    <t>OncoScan.FFPE.na33.r1.REF_MODEL</t>
+  </si>
+  <si>
+    <t>OncoScan.na33.r1.annot.db</t>
+  </si>
+  <si>
+    <t>OncoScan.r1.chrYprobes</t>
+  </si>
+  <si>
+    <t>OncoScan.r1.chrXprobes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OncoScan.r1.snplist.txt </t>
+  </si>
+  <si>
+    <t>custom</t>
+  </si>
+  <si>
+    <t>C:\Users\e.bordron\Desktop\CGH-scoring\library_files_oncoscan\OncoScan_Array_analysis_Files_NA33-r3</t>
+  </si>
+  <si>
+    <t>input of 
+apt-copynumber-onco-ssa</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fichier texte à 4 colonnes ayant pour lignes les sondes. Besoin du fichier CDF d'oncoscan -&gt; Tony Sierra
+OU
+d'utiliser apt-copynumber-onco-ssa -&gt; télécharger apt
+OU
+d'utiliser apt.oncoscan.2.4.0, une sous-partie d'EaCoN. -&gt; linux
+</t>
+  </si>
+  <si>
+    <t>valeurs LRR (CGHcall utilise les informations de breakpoint (par l'algo CBS, typiquement). Cela est envoyé vers un objet R: cghSeg
 https://www.rdocumentation.org/packages/CGHbase/versions/1.32.0/topics/cghSeg</t>
   </si>
   <si>
-    <t>need of cnchp files</t>
+    <t>classifie le LRR entre ref et tumeur en 5 états: double loss-homozygous (biallelic) deletion, loss-hemizygous deletion (loss of one of the alleles), normal-two copies, gain-three to four copies and amplification–more than four copies</t>
+  </si>
+  <si>
+    <t>résolution</t>
+  </si>
+  <si>
+    <t>calcul de différents scores de HRD</t>
+  </si>
+  <si>
+    <t>spécificité du package</t>
+  </si>
+  <si>
+    <t>système de visualisation interactive des données</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - prend en compte la cellularité (on la renseigne)
+- un mixture model est utilisé (outil de clustering statistique)
+- </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -765,8 +888,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -782,6 +917,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -809,7 +950,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -857,11 +998,37 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -884,8 +1051,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>306324</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1916049</xdr:colOff>
       <xdr:row>63</xdr:row>
       <xdr:rowOff>29672</xdr:rowOff>
     </xdr:to>
@@ -1010,6 +1177,20 @@
     <tableColumn id="4" name="End Position"/>
     <tableColumn id="5" name="Num Markers"/>
     <tableColumn id="6" name="Seg.CN"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tableau7" displayName="Tableau7" ref="B89:F95" totalsRowShown="0">
+  <autoFilter ref="B89:F95"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="2" name="File extension/type"/>
+    <tableColumn id="3" name="Description"/>
+    <tableColumn id="4" name="where to find it"/>
+    <tableColumn id="5" name="Actual name" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1283,8 +1464,8 @@
   </sheetPr>
   <dimension ref="A1:AC137"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,7 +1476,7 @@
     <col min="4" max="4" width="72.7109375" style="11" customWidth="1"/>
     <col min="5" max="5" width="41.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="50.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="33.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" style="4" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="4"/>
     <col min="10" max="10" width="12" style="4" customWidth="1"/>
@@ -1321,12 +1502,14 @@
         <v>5</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="4"/>
+      <c r="G1" s="3" t="s">
+        <v>215</v>
+      </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -1355,21 +1538,23 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="G2" s="4"/>
+        <v>110</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>214</v>
+      </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -1398,21 +1583,21 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G3" s="4"/>
+        <v>111</v>
+      </c>
+      <c r="G3" s="3"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -1436,26 +1621,28 @@
       <c r="AB3" s="4"/>
       <c r="AC3" s="4"/>
     </row>
-    <row r="4" spans="1:29" s="8" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" s="8" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>126</v>
+        <v>210</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G4" s="4"/>
+        <v>116</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>216</v>
+      </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -1481,28 +1668,33 @@
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B5" s="3"/>
+        <v>117</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>209</v>
+      </c>
       <c r="C5" s="16" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" s="7"/>
+        <v>118</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>209</v>
+      </c>
       <c r="C6" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="4"/>
+      <c r="G6" s="6"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -1528,28 +1720,33 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B7" s="9"/>
+        <v>119</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>209</v>
+      </c>
       <c r="C7" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:29" s="8" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B8" s="7"/>
+        <v>120</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>209</v>
+      </c>
       <c r="C8" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
-      <c r="G8" s="4"/>
+      <c r="G8" s="6"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -1573,17 +1770,24 @@
       <c r="AB8" s="4"/>
       <c r="AC8" s="4"/>
     </row>
-    <row r="9" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B9" s="9"/>
+        <v>121</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>209</v>
+      </c>
       <c r="C9" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="D9" s="9"/>
+        <v>211</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>212</v>
+      </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
+      <c r="G9" s="9" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
@@ -1628,7 +1832,7 @@
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
+      <c r="C15" s="19"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -1660,7 +1864,9 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
+      <c r="C19" s="10" t="s">
+        <v>217</v>
+      </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
@@ -2611,19 +2817,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="48" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="43" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A3:P86"/>
+  <dimension ref="A3:P95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F88" sqref="F88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2631,9 +2837,9 @@
     <col min="1" max="1" width="24.85546875" style="14" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
@@ -2656,69 +2862,69 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>14</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>15</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>16</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>17</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>18</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>19</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>20</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>21</v>
-      </c>
-      <c r="P4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="F5" s="1">
         <v>58858172</v>
@@ -2730,43 +2936,45 @@
         <v>16043</v>
       </c>
       <c r="I5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" t="s">
         <v>31</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>32</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>33</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>34</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>35</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>36</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>37</v>
       </c>
-      <c r="P5" t="s">
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" s="1">
         <v>58859117</v>
@@ -2775,46 +2983,46 @@
         <v>58866549</v>
       </c>
       <c r="H6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" t="s">
         <v>41</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P6" t="s">
         <v>42</v>
-      </c>
-      <c r="J6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6" t="s">
-        <v>33</v>
-      </c>
-      <c r="L6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N6" t="s">
-        <v>36</v>
-      </c>
-      <c r="O6" t="s">
-        <v>37</v>
-      </c>
-      <c r="P6" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="F7" s="1">
         <v>52559169</v>
@@ -2826,28 +3034,28 @@
         <v>86267</v>
       </c>
       <c r="I7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J7" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" t="s">
         <v>48</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>49</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>50</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
+        <v>35</v>
+      </c>
+      <c r="O7" t="s">
+        <v>36</v>
+      </c>
+      <c r="P7" t="s">
         <v>51</v>
-      </c>
-      <c r="N7" t="s">
-        <v>36</v>
-      </c>
-      <c r="O7" t="s">
-        <v>37</v>
-      </c>
-      <c r="P7" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -2876,216 +3084,216 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" t="s">
         <v>57</v>
       </c>
-      <c r="F11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>58</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>59</v>
       </c>
-      <c r="I11" t="s">
-        <v>60</v>
-      </c>
       <c r="J11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="E12" s="1">
         <v>249116709</v>
       </c>
       <c r="F12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" t="s">
         <v>64</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>65</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>66</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>67</v>
-      </c>
-      <c r="J12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="E13" s="1">
         <v>242497851</v>
       </c>
       <c r="F13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" t="s">
         <v>71</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>72</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>73</v>
       </c>
-      <c r="I13" t="s">
-        <v>74</v>
-      </c>
       <c r="J13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="E14" s="1">
         <v>197683938</v>
       </c>
       <c r="F14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" t="s">
         <v>77</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
+        <v>72</v>
+      </c>
+      <c r="I14" t="s">
         <v>78</v>
       </c>
-      <c r="H14" t="s">
-        <v>73</v>
-      </c>
-      <c r="I14" t="s">
-        <v>79</v>
-      </c>
       <c r="J14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="E15" s="1">
         <v>190921709</v>
       </c>
       <c r="F15" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" t="s">
         <v>82</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" t="s">
         <v>83</v>
       </c>
-      <c r="H15" t="s">
-        <v>66</v>
-      </c>
-      <c r="I15" t="s">
-        <v>84</v>
-      </c>
       <c r="J15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="E16" s="1">
         <v>180579439</v>
       </c>
       <c r="F16" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" t="s">
         <v>87</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
+        <v>72</v>
+      </c>
+      <c r="I16" t="s">
         <v>88</v>
       </c>
-      <c r="H16" t="s">
-        <v>73</v>
-      </c>
-      <c r="I16" t="s">
-        <v>89</v>
-      </c>
       <c r="J16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="E17" s="1">
         <v>170849100</v>
       </c>
       <c r="F17" t="s">
+        <v>91</v>
+      </c>
+      <c r="G17" t="s">
         <v>92</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
+        <v>65</v>
+      </c>
+      <c r="I17" t="s">
         <v>93</v>
       </c>
-      <c r="H17" t="s">
-        <v>66</v>
-      </c>
-      <c r="I17" t="s">
-        <v>94</v>
-      </c>
       <c r="J17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -3114,60 +3322,60 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>98</v>
+        <v>177</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -3196,40 +3404,40 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B67" t="s">
+        <v>126</v>
+      </c>
+      <c r="C67" t="s">
+        <v>127</v>
+      </c>
+      <c r="D67" t="s">
         <v>128</v>
       </c>
-      <c r="C67" t="s">
-        <v>129</v>
-      </c>
-      <c r="D67" t="s">
-        <v>130</v>
-      </c>
       <c r="E67" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F67" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B68" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C68">
         <v>6</v>
@@ -3238,18 +3446,18 @@
         <v>94609</v>
       </c>
       <c r="E68" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F68" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G68" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C69">
         <v>6</v>
@@ -3258,18 +3466,18 @@
         <v>110632</v>
       </c>
       <c r="E69" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F69" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G69" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C70">
         <v>6</v>
@@ -3278,18 +3486,18 @@
         <v>133969</v>
       </c>
       <c r="E70" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F70" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G70" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C71">
         <v>6</v>
@@ -3298,38 +3506,38 @@
         <v>151528</v>
       </c>
       <c r="E71" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F71" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G71" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B74" t="s">
+        <v>151</v>
+      </c>
+      <c r="C74" t="s">
         <v>152</v>
       </c>
-      <c r="B74" t="s">
+      <c r="D74" t="s">
         <v>153</v>
       </c>
-      <c r="C74" t="s">
-        <v>154</v>
-      </c>
-      <c r="D74" t="s">
-        <v>155</v>
-      </c>
       <c r="E74" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B75" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -3343,7 +3551,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C76">
         <v>19</v>
@@ -3357,30 +3565,33 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="B79" t="s">
+        <v>159</v>
+      </c>
+      <c r="C79" t="s">
+        <v>160</v>
+      </c>
+      <c r="D79" t="s">
+        <v>170</v>
+      </c>
+      <c r="E79" t="s">
+        <v>171</v>
+      </c>
+      <c r="F79" t="s">
+        <v>172</v>
+      </c>
+      <c r="G79" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="B79" t="s">
-        <v>161</v>
-      </c>
-      <c r="C79" t="s">
+      <c r="B80" t="s">
         <v>162</v>
-      </c>
-      <c r="D79" t="s">
-        <v>172</v>
-      </c>
-      <c r="E79" t="s">
-        <v>173</v>
-      </c>
-      <c r="F79" t="s">
-        <v>174</v>
-      </c>
-      <c r="G79" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>164</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -3395,12 +3606,12 @@
         <v>2632</v>
       </c>
       <c r="G80" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -3415,12 +3626,12 @@
         <v>2</v>
       </c>
       <c r="G81" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -3435,12 +3646,12 @@
         <v>2075</v>
       </c>
       <c r="G82" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -3455,12 +3666,12 @@
         <v>4494</v>
       </c>
       <c r="G83" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C84">
         <v>2</v>
@@ -3475,12 +3686,12 @@
         <v>1950</v>
       </c>
       <c r="G84" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C85">
         <v>2</v>
@@ -3495,12 +3706,12 @@
         <v>2</v>
       </c>
       <c r="G85" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C86">
         <v>2</v>
@@ -3515,20 +3726,147 @@
         <v>5505</v>
       </c>
       <c r="G86" t="s">
-        <v>171</v>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="B89" t="s">
+        <v>151</v>
+      </c>
+      <c r="C89" t="s">
+        <v>179</v>
+      </c>
+      <c r="D89" t="s">
+        <v>180</v>
+      </c>
+      <c r="E89" t="s">
+        <v>107</v>
+      </c>
+      <c r="F89" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="B90" t="s">
+        <v>181</v>
+      </c>
+      <c r="C90" t="s">
+        <v>182</v>
+      </c>
+      <c r="D90" t="s">
+        <v>183</v>
+      </c>
+      <c r="E90" t="s">
+        <v>207</v>
+      </c>
+      <c r="F90" s="17" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>184</v>
+      </c>
+      <c r="C91" t="s">
+        <v>185</v>
+      </c>
+      <c r="D91" t="s">
+        <v>186</v>
+      </c>
+      <c r="E91" t="s">
+        <v>207</v>
+      </c>
+      <c r="F91" s="18" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>187</v>
+      </c>
+      <c r="C92" t="s">
+        <v>188</v>
+      </c>
+      <c r="D92" t="s">
+        <v>189</v>
+      </c>
+      <c r="E92" t="s">
+        <v>207</v>
+      </c>
+      <c r="F92" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>190</v>
+      </c>
+      <c r="C93" t="s">
+        <v>191</v>
+      </c>
+      <c r="D93" t="s">
+        <v>192</v>
+      </c>
+      <c r="E93" t="s">
+        <v>207</v>
+      </c>
+      <c r="F93" s="17" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>193</v>
+      </c>
+      <c r="C94" t="s">
+        <v>194</v>
+      </c>
+      <c r="D94" t="s">
+        <v>195</v>
+      </c>
+      <c r="E94" t="s">
+        <v>207</v>
+      </c>
+      <c r="F94" s="17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>196</v>
+      </c>
+      <c r="C95" t="s">
+        <v>197</v>
+      </c>
+      <c r="D95" t="s">
+        <v>198</v>
+      </c>
+      <c r="E95" t="s">
+        <v>206</v>
+      </c>
+      <c r="F95" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="55" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="6">
-    <tablePart r:id="rId3"/>
+  <legacyDrawing r:id="rId3"/>
+  <tableParts count="7">
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>